<commit_message>
Mise à jour des fichiers DOC pour le premier dépôt vers Mr Martiel
</commit_message>
<xml_diff>
--- a/ShopConnect_Echeancier.xlsx
+++ b/ShopConnect_Echeancier.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a_StLaurent\DOC_ISL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ShopConnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2211D8-3A3A-4E38-8E45-402B4A77D9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EB3DC0-12A1-4DB2-B9FE-F00DF6C610E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -875,17 +875,533 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="212">
+  <dxfs count="209">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF9900"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF9900"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF9900"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF9900"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF9900"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF9900"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF9900"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFF2CC"/>
@@ -899,76 +1415,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF9900"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF34A853"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FFFFF2CC"/>
       </font>
       <fill>
@@ -1002,458 +1448,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF9900"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF34A853"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF9900"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF34A853"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF9900"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF34A853"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF9900"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF34A853"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF9900"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF34A853"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF9900"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF34A853"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FFFFF2CC"/>
       </font>
       <fill>
@@ -1493,6 +1487,947 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF8989EB"/>
           <bgColor rgb="FF8989EB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF073763"/>
+        </left>
+        <top style="thick">
+          <color rgb="FF073763"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF073763"/>
+        </left>
+        <top style="thick">
+          <color rgb="FF073763"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF073763"/>
+        </left>
+        <top style="thick">
+          <color rgb="FF073763"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF073763"/>
+        </left>
+        <top style="thick">
+          <color rgb="FF073763"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1525,820 +2460,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="mediumDashDot">
-          <color rgb="FF92D050"/>
-        </left>
-        <right style="mediumDashDot">
-          <color rgb="FF92D050"/>
-        </right>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="mediumDashDot">
-          <color rgb="FF92D050"/>
-        </left>
-        <right style="mediumDashDot">
-          <color rgb="FF92D050"/>
-        </right>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF073763"/>
-        </left>
-        <top style="thick">
-          <color rgb="FF073763"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF073763"/>
-        </left>
-        <top style="thick">
-          <color rgb="FF073763"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF073763"/>
-        </left>
-        <top style="thick">
-          <color rgb="FF073763"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF073763"/>
-        </left>
-        <top style="thick">
-          <color rgb="FF073763"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2680,6 +2801,40 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="mediumDashDot">
           <color rgb="FF92D050"/>
@@ -3339,209 +3494,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="mediumDashDot">
-          <color rgb="FF92D050"/>
-        </left>
-        <right style="mediumDashDot">
-          <color rgb="FF92D050"/>
-        </right>
-        <top style="mediumDashDot">
-          <color rgb="FF92D050"/>
-        </top>
-        <bottom style="mediumDashDot">
-          <color rgb="FF92D050"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
@@ -3712,39 +3664,39 @@
   </dxfs>
   <tableStyles count="7">
     <tableStyle name="Echéancier-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="211"/>
-      <tableStyleElement type="firstRowStripe" dxfId="210"/>
-      <tableStyleElement type="secondRowStripe" dxfId="209"/>
-    </tableStyle>
-    <tableStyle name="Echéancier-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="208"/>
       <tableStyleElement type="firstRowStripe" dxfId="207"/>
       <tableStyleElement type="secondRowStripe" dxfId="206"/>
     </tableStyle>
-    <tableStyle name="Echéancier-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+    <tableStyle name="Echéancier-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="205"/>
       <tableStyleElement type="firstRowStripe" dxfId="204"/>
       <tableStyleElement type="secondRowStripe" dxfId="203"/>
     </tableStyle>
-    <tableStyle name="Echéancier-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
+    <tableStyle name="Echéancier-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
       <tableStyleElement type="headerRow" dxfId="202"/>
       <tableStyleElement type="firstRowStripe" dxfId="201"/>
       <tableStyleElement type="secondRowStripe" dxfId="200"/>
     </tableStyle>
-    <tableStyle name="Echéancier-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
+    <tableStyle name="Echéancier-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
       <tableStyleElement type="headerRow" dxfId="199"/>
       <tableStyleElement type="firstRowStripe" dxfId="198"/>
       <tableStyleElement type="secondRowStripe" dxfId="197"/>
     </tableStyle>
-    <tableStyle name="Echéancier-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
+    <tableStyle name="Echéancier-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
       <tableStyleElement type="headerRow" dxfId="196"/>
       <tableStyleElement type="firstRowStripe" dxfId="195"/>
       <tableStyleElement type="secondRowStripe" dxfId="194"/>
     </tableStyle>
-    <tableStyle name="Echéancier-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
+    <tableStyle name="Echéancier-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
       <tableStyleElement type="headerRow" dxfId="193"/>
       <tableStyleElement type="firstRowStripe" dxfId="192"/>
       <tableStyleElement type="secondRowStripe" dxfId="191"/>
+    </tableStyle>
+    <tableStyle name="Echéancier-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
+      <tableStyleElement type="headerRow" dxfId="190"/>
+      <tableStyleElement type="firstRowStripe" dxfId="189"/>
+      <tableStyleElement type="secondRowStripe" dxfId="188"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3767,16 +3719,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="B3:I4" headerRowCount="0" headerRowDxfId="190" dataDxfId="189" totalsRowDxfId="187" tableBorderDxfId="188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="B3:I4" headerRowCount="0" headerRowDxfId="187" dataDxfId="186" totalsRowDxfId="184" tableBorderDxfId="185">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="186"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="185"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="184"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataDxfId="183"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="182"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="181"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="180"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="177"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="176"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3788,32 +3740,32 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D7055961-3976-404E-A8A0-FE37D3AF2824}" name="Table_7111314" displayName="Table_7111314" ref="B42:I46" headerRowCount="0" headerRowDxfId="85" dataDxfId="84" totalsRowDxfId="82" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D7055961-3976-404E-A8A0-FE37D3AF2824}" name="Table_7111314" displayName="Table_7111314" ref="B42:I46" headerRowCount="0" headerRowDxfId="79" dataDxfId="78" totalsRowDxfId="76" tableBorderDxfId="77">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4F37DEBE-CD3F-47FB-B28E-0EBB6D97E99E}" name="Column1" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{7340370D-E9FC-47EB-98D4-E5CA0F9AA699}" name="Column2" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{DE74EB65-C08C-4175-938C-EAB2D5378666}" name="Column3" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{0BFA89BF-1C2D-496C-B570-E6B427752F35}" name="Column4" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{B67EA5E1-1F31-4A96-AFBB-69EE9D46FEFD}" name="Column5" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{0AA4955D-86AD-4E7E-A518-735EAB12E64E}" name="Column6" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{35969E28-2F6D-452E-A5C7-5F65CBEB5265}" name="Column7" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{AE06E83D-85AC-47DA-9943-EBBFAD5CF315}" name="Column8" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{4F37DEBE-CD3F-47FB-B28E-0EBB6D97E99E}" name="Column1" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{7340370D-E9FC-47EB-98D4-E5CA0F9AA699}" name="Column2" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{DE74EB65-C08C-4175-938C-EAB2D5378666}" name="Column3" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{0BFA89BF-1C2D-496C-B570-E6B427752F35}" name="Column4" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{B67EA5E1-1F31-4A96-AFBB-69EE9D46FEFD}" name="Column5" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{0AA4955D-86AD-4E7E-A518-735EAB12E64E}" name="Column6" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{35969E28-2F6D-452E-A5C7-5F65CBEB5265}" name="Column7" dataDxfId="69"/>
+    <tableColumn id="8" xr3:uid="{AE06E83D-85AC-47DA-9943-EBBFAD5CF315}" name="Column8" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="B5:I6" headerRowCount="0" headerRowDxfId="178" dataDxfId="177" totalsRowDxfId="175" tableBorderDxfId="176">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="B5:I6" headerRowCount="0" headerRowDxfId="175" dataDxfId="174" totalsRowDxfId="172" tableBorderDxfId="173">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="174"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" dataDxfId="173"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column3" dataDxfId="172"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column4" dataDxfId="171"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Column5" dataDxfId="170"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Column6" dataDxfId="169"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Column7" dataDxfId="168"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Column8" dataDxfId="167"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="171"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" dataDxfId="170"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column3" dataDxfId="169"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column4" dataDxfId="168"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Column5" dataDxfId="167"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Column6" dataDxfId="166"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Column7" dataDxfId="165"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Column8" dataDxfId="164"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3825,16 +3777,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="B7:I10" headerRowCount="0" headerRowDxfId="166" dataDxfId="165" totalsRowDxfId="163" tableBorderDxfId="164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="B7:I10" headerRowCount="0" headerRowDxfId="163" dataDxfId="162" totalsRowDxfId="160" tableBorderDxfId="161">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Column2" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Column3" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column4" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Column5" dataDxfId="158"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Column6" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Column7" dataDxfId="156"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Column8" dataDxfId="155"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="159"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Column2" dataDxfId="158"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Column3" dataDxfId="157"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column4" dataDxfId="156"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Column5" dataDxfId="155"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Column6" dataDxfId="154"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Column7" dataDxfId="153"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Column8" dataDxfId="152"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3846,16 +3798,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="B11:I14" headerRowCount="0" headerRowDxfId="154" dataDxfId="153" totalsRowDxfId="151" tableBorderDxfId="152">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="B11:I14" headerRowCount="0" headerRowDxfId="151" dataDxfId="150" totalsRowDxfId="148" tableBorderDxfId="149">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Column3" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Column4" dataDxfId="147"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Column5" dataDxfId="146"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Column6" dataDxfId="145"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Column7" dataDxfId="144"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Column8" dataDxfId="143"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="147"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2" dataDxfId="146"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Column3" dataDxfId="145"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Column4" dataDxfId="144"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Column5" dataDxfId="143"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Column6" dataDxfId="142"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Column7" dataDxfId="141"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Column8" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3867,16 +3819,16 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="B15:I18" headerRowCount="0" headerRowDxfId="142" dataDxfId="141" totalsRowDxfId="139" tableBorderDxfId="140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_5" displayName="Table_5" ref="B15:I18" headerRowCount="0" headerRowDxfId="139" dataDxfId="138" totalsRowDxfId="136" tableBorderDxfId="137">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1" dataDxfId="138"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Column2" dataDxfId="137"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Column3" dataDxfId="136"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Column4" dataDxfId="135"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Column5" dataDxfId="134"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Column6" dataDxfId="133"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Column7" dataDxfId="132"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Column8" dataDxfId="131"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Column2" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Column3" dataDxfId="133"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Column4" dataDxfId="132"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Column5" dataDxfId="131"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Column6" dataDxfId="130"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Column7" dataDxfId="129"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Column8" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3888,16 +3840,16 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="B22:I23" headerRowCount="0" headerRowDxfId="71" dataDxfId="70" totalsRowDxfId="69" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_6" displayName="Table_6" ref="B22:I23" headerRowCount="0" headerRowDxfId="127" dataDxfId="126" totalsRowDxfId="124" tableBorderDxfId="125">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Column1" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Column2" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Column3" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Column4" dataDxfId="126"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Column5" dataDxfId="125"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Column6" dataDxfId="124"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Column7" dataDxfId="123"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Column8" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Column1" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Column2" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Column3" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Column4" dataDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Column5" dataDxfId="119"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Column6" dataDxfId="118"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Column7" dataDxfId="117"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Column8" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3909,16 +3861,16 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_7" displayName="Table_7" ref="B25:I29" headerRowCount="0" headerRowDxfId="121" dataDxfId="120" totalsRowDxfId="118" tableBorderDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_7" displayName="Table_7" ref="B25:I29" headerRowCount="0" headerRowDxfId="115" dataDxfId="114" totalsRowDxfId="112" tableBorderDxfId="113">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Column1" dataDxfId="117"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Column2" dataDxfId="116"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Column3" dataDxfId="115"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Column4" dataDxfId="114"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Column5" dataDxfId="113"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Column6" dataDxfId="112"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Column7" dataDxfId="111"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Column8" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Column1" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Column2" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Column3" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Column4" dataDxfId="108"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Column5" dataDxfId="107"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Column6" dataDxfId="106"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Column7" dataDxfId="105"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Column8" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3930,32 +3882,32 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{59DA55F3-B6F5-4A28-AF65-BF025DABF206}" name="Table_711" displayName="Table_711" ref="B30:I35" headerRowCount="0" headerRowDxfId="109" dataDxfId="108" totalsRowDxfId="106" tableBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{59DA55F3-B6F5-4A28-AF65-BF025DABF206}" name="Table_711" displayName="Table_711" ref="B30:I35" headerRowCount="0" headerRowDxfId="103" dataDxfId="102" totalsRowDxfId="100" tableBorderDxfId="101">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B7A86860-E288-4C5A-87E4-DDC684CD85EA}" name="Column1" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{41F147C3-7EA0-4372-8F4E-CC9CA1553540}" name="Column2" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{225E73ED-C3FD-4FB6-8648-9DAD9659936F}" name="Column3" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{51AA7878-3DBD-4B07-A142-9A35B1C76D46}" name="Column4" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{3FE4AFD6-AD92-4C33-8C0B-30198B118B7D}" name="Column5" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{58CB6DB8-DD9F-4A25-AEA7-4A398A1F86FD}" name="Column6" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{C1616B17-96B8-49A1-8A4C-93E447BE19C9}" name="Column7" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{7039DCEF-21B8-4190-B8AA-6A76E5AF4420}" name="Column8" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{B7A86860-E288-4C5A-87E4-DDC684CD85EA}" name="Column1" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{41F147C3-7EA0-4372-8F4E-CC9CA1553540}" name="Column2" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{225E73ED-C3FD-4FB6-8648-9DAD9659936F}" name="Column3" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{51AA7878-3DBD-4B07-A142-9A35B1C76D46}" name="Column4" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{3FE4AFD6-AD92-4C33-8C0B-30198B118B7D}" name="Column5" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{58CB6DB8-DD9F-4A25-AEA7-4A398A1F86FD}" name="Column6" dataDxfId="94"/>
+    <tableColumn id="7" xr3:uid="{C1616B17-96B8-49A1-8A4C-93E447BE19C9}" name="Column7" dataDxfId="93"/>
+    <tableColumn id="8" xr3:uid="{7039DCEF-21B8-4190-B8AA-6A76E5AF4420}" name="Column8" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4998C22D-B653-47A5-BFBA-5B4FD4FAAF94}" name="Table_71113" displayName="Table_71113" ref="B36:I41" headerRowCount="0" headerRowDxfId="97" dataDxfId="96" totalsRowDxfId="94" tableBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4998C22D-B653-47A5-BFBA-5B4FD4FAAF94}" name="Table_71113" displayName="Table_71113" ref="B36:I41" headerRowCount="0" headerRowDxfId="91" dataDxfId="90" totalsRowDxfId="88" tableBorderDxfId="89">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B3CE7581-EB45-4252-A092-770D188C11DB}" name="Column1" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{3E75E14F-2598-45A8-BBC8-D7EAF32C55D6}" name="Column2" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{4072D6AD-D606-4BF2-959E-E5E24C405796}" name="Column3" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{D89EB40C-A3D2-4ABD-8A93-17CE2FE8A321}" name="Column4" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{E8C69047-FB2F-4EFB-89D9-131D2F9179CC}" name="Column5" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{8FD039AA-2826-4421-8C9C-52255DACA09C}" name="Column6" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{863441B5-AD0B-4904-916A-198D85FBD300}" name="Column7" dataDxfId="87"/>
-    <tableColumn id="8" xr3:uid="{5E781CAE-AF89-4F91-859B-611F1AC60B2C}" name="Column8" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{B3CE7581-EB45-4252-A092-770D188C11DB}" name="Column1" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{3E75E14F-2598-45A8-BBC8-D7EAF32C55D6}" name="Column2" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{4072D6AD-D606-4BF2-959E-E5E24C405796}" name="Column3" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{D89EB40C-A3D2-4ABD-8A93-17CE2FE8A321}" name="Column4" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{E8C69047-FB2F-4EFB-89D9-131D2F9179CC}" name="Column5" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{8FD039AA-2826-4421-8C9C-52255DACA09C}" name="Column6" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{863441B5-AD0B-4904-916A-198D85FBD300}" name="Column7" dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{5E781CAE-AF89-4F91-859B-611F1AC60B2C}" name="Column8" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4594,8 +4546,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B22" s="56" t="s">
+    <row r="22" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="8"/>
@@ -4604,9 +4556,9 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="57"/>
+      <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
         <v>17</v>
       </c>
@@ -4630,7 +4582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:9" s="2" customFormat="1" ht="13.8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" s="2" customFormat="1" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B24" s="49"/>
       <c r="C24" s="16"/>
       <c r="D24" s="17"/>
@@ -4640,8 +4592,8 @@
       <c r="H24" s="19"/>
       <c r="I24" s="50"/>
     </row>
-    <row r="25" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B25" s="56" t="s">
+    <row r="25" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="8"/>
@@ -4650,9 +4602,9 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="57"/>
+      <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="2:9" s="2" customFormat="1" ht="28.2" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" s="2" customFormat="1" ht="28.2" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="44" t="s">
         <v>58</v>
       </c>
@@ -4676,7 +4628,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="31" t="s">
         <v>31</v>
       </c>
@@ -4688,7 +4640,7 @@
       <c r="H27" s="33"/>
       <c r="I27" s="34"/>
     </row>
-    <row r="28" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B28" s="36" t="s">
         <v>61</v>
       </c>
@@ -4712,7 +4664,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="2:9" s="2" customFormat="1" ht="42" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" s="2" customFormat="1" ht="42" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="38" t="s">
         <v>64</v>
       </c>
@@ -4736,7 +4688,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="31" t="s">
         <v>32</v>
       </c>
@@ -4748,7 +4700,7 @@
       <c r="H30" s="33"/>
       <c r="I30" s="34"/>
     </row>
-    <row r="31" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B31" s="45" t="s">
         <v>67</v>
       </c>
@@ -4772,7 +4724,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="2:9" s="2" customFormat="1" ht="28.2" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" s="2" customFormat="1" ht="28.2" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="38" t="s">
         <v>70</v>
       </c>
@@ -4796,7 +4748,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="31" t="s">
         <v>33</v>
       </c>
@@ -4808,7 +4760,7 @@
       <c r="H33" s="33"/>
       <c r="I33" s="34"/>
     </row>
-    <row r="34" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B34" s="45" t="s">
         <v>73</v>
       </c>
@@ -4832,7 +4784,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="2:9" s="2" customFormat="1" ht="14.4" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" s="2" customFormat="1" ht="14.4" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="38" t="s">
         <v>21</v>
       </c>
@@ -4852,7 +4804,7 @@
       <c r="H35" s="42"/>
       <c r="I35" s="43"/>
     </row>
-    <row r="36" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="31" t="s">
         <v>34</v>
       </c>
@@ -4864,7 +4816,7 @@
       <c r="H36" s="33"/>
       <c r="I36" s="34"/>
     </row>
-    <row r="37" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B37" s="36" t="s">
         <v>76</v>
       </c>
@@ -4888,7 +4840,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="2:9" s="2" customFormat="1" ht="28.2" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" s="2" customFormat="1" ht="28.2" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="38" t="s">
         <v>40</v>
       </c>
@@ -4908,7 +4860,7 @@
       <c r="H38" s="42"/>
       <c r="I38" s="43"/>
     </row>
-    <row r="39" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="31" t="s">
         <v>35</v>
       </c>
@@ -4920,7 +4872,7 @@
       <c r="H39" s="33"/>
       <c r="I39" s="34"/>
     </row>
-    <row r="40" spans="2:9" s="2" customFormat="1" ht="27.6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" s="2" customFormat="1" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B40" s="36" t="s">
         <v>18</v>
       </c>
@@ -4944,7 +4896,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="2:9" s="2" customFormat="1" ht="14.4" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" s="2" customFormat="1" ht="14.4" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="38"/>
       <c r="C41" s="39"/>
       <c r="D41" s="40" t="s">
@@ -4958,7 +4910,7 @@
       <c r="H41" s="42"/>
       <c r="I41" s="43"/>
     </row>
-    <row r="42" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="31" t="s">
         <v>36</v>
       </c>
@@ -4970,7 +4922,7 @@
       <c r="H42" s="33"/>
       <c r="I42" s="34"/>
     </row>
-    <row r="43" spans="2:9" s="2" customFormat="1" ht="28.2" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" s="2" customFormat="1" ht="28.2" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="38" t="s">
         <v>79</v>
       </c>
@@ -4994,7 +4946,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="31" t="s">
         <v>37</v>
       </c>
@@ -5006,7 +4958,7 @@
       <c r="H44" s="33"/>
       <c r="I44" s="34"/>
     </row>
-    <row r="45" spans="2:9" s="2" customFormat="1" ht="42" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" s="2" customFormat="1" ht="42" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="38" t="s">
         <v>82</v>
       </c>
@@ -5030,7 +4982,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" collapsed="1" x14ac:dyDescent="0.3">
       <c r="B46" s="31" t="s">
         <v>38</v>
       </c>
@@ -5042,7 +4994,7 @@
       <c r="H46" s="33"/>
       <c r="I46" s="34"/>
     </row>
-    <row r="47" spans="2:9" s="2" customFormat="1" ht="42" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" s="2" customFormat="1" ht="42" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="38" t="s">
         <v>85</v>
       </c>
@@ -5070,262 +5022,262 @@
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="67" priority="156" operator="equal">
+  <conditionalFormatting sqref="B23">
+    <cfRule type="cellIs" dxfId="67" priority="13" operator="equal">
+      <formula>"Groupe UI"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="cellIs" dxfId="66" priority="12" operator="equal">
       <formula>"Groupe UI"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="cellIs" dxfId="66" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="20" operator="equal">
       <formula>"Groupe UI"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="65" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="17" operator="equal">
       <formula>"Groupe UI"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:B38">
-    <cfRule type="cellIs" dxfId="64" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="83" operator="equal">
       <formula>"Groupe UI"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2 D4 D6 D26 D8:D10 D23:D24 D20:D21 D16:D18 D12:D14">
-    <cfRule type="cellIs" dxfId="63" priority="143" operator="equal">
+  <conditionalFormatting sqref="B43">
+    <cfRule type="cellIs" dxfId="62" priority="2" operator="equal">
+      <formula>"Groupe UI"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
+      <formula>"Groupe UI"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="cellIs" dxfId="60" priority="156" operator="equal">
+      <formula>"Groupe UI"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2 D4 D6 D8:D10 D12:D14 D16:D18 D20:D21 D23:D24 D26">
+    <cfRule type="cellIs" dxfId="59" priority="143" operator="equal">
       <formula>"Terminé(e)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="144" operator="equal">
       <formula>"En cours"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 D6 D26 D8:D10 D23:D24 D20:D21 D16:D18 D12:D14">
-    <cfRule type="cellIs" dxfId="61" priority="145" operator="equal">
+  <conditionalFormatting sqref="D4 D6 D8:D10 D12:D14 D16:D18 D20:D21 D23:D24 D26">
+    <cfRule type="cellIs" dxfId="57" priority="147" operator="equal">
+      <formula>"À tester"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="146" operator="equal">
+      <formula>"Abandonné"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="145" operator="equal">
       <formula>"À faire"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="146" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D29 D45 D47">
+    <cfRule type="cellIs" dxfId="54" priority="39" operator="equal">
+      <formula>"En cours"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="40" operator="equal">
+      <formula>"À faire"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="41" operator="equal">
       <formula>"Abandonné"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="42" operator="equal">
       <formula>"À tester"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D29 D47 D45">
-    <cfRule type="cellIs" dxfId="58" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="38" operator="equal">
       <formula>"Terminé(e)"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="39" operator="equal">
-      <formula>"En cours"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
-      <formula>"À faire"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="41" operator="equal">
-      <formula>"Abandonné"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="42" operator="equal">
-      <formula>"À tester"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D32">
-    <cfRule type="cellIs" dxfId="53" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
+      <formula>"À faire"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="21" operator="equal">
       <formula>"Terminé(e)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="22" operator="equal">
       <formula>"En cours"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="23" operator="equal">
-      <formula>"À faire"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
       <formula>"Abandonné"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="25" operator="equal">
       <formula>"À tester"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:D35">
-    <cfRule type="cellIs" dxfId="48" priority="111" operator="equal">
-      <formula>"Terminé(e)"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="112" operator="equal">
-      <formula>"En cours"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="113" operator="equal">
-      <formula>"À faire"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="114" operator="equal">
-      <formula>"Abandonné"</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="44" priority="115" operator="equal">
       <formula>"À tester"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="113" operator="equal">
+      <formula>"À faire"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="111" operator="equal">
+      <formula>"Terminé(e)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="112" operator="equal">
+      <formula>"En cours"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="114" operator="equal">
+      <formula>"Abandonné"</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D38">
-    <cfRule type="cellIs" dxfId="43" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="85" operator="equal">
+      <formula>"En cours"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="84" operator="equal">
       <formula>"Terminé(e)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="85" operator="equal">
-      <formula>"En cours"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="86" operator="equal">
       <formula>"À faire"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="87" operator="equal">
       <formula>"Abandonné"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="88" operator="equal">
       <formula>"À tester"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:D41">
-    <cfRule type="cellIs" dxfId="38" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="75" operator="equal">
+      <formula>"En cours"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="78" operator="equal">
+      <formula>"À tester"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="74" operator="equal">
       <formula>"Terminé(e)"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="76" operator="equal">
+      <formula>"À faire"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="77" operator="equal">
+      <formula>"Abandonné"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+      <formula>"Terminé(e)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"En cours"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>"À faire"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>"Abandonné"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"À tester"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4 E6 E8:E10 E12:E14 E16:E18 E20:E21 E23:E24 E26 E45 E47">
+    <cfRule type="cellIs" dxfId="24" priority="150" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="149" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="148" operator="equal">
+      <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 E14">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="158">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="158">
       <formula>LEN(TRIM(E10))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26 E4 E6 E8:E10 E23:E24 E47 E45 E20:E21 E16:E18 E12:E14">
-    <cfRule type="cellIs" dxfId="32" priority="148" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="149" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="150" operator="equal">
-      <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="46">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="46">
       <formula>LEN(TRIM(E28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E29">
-    <cfRule type="cellIs" dxfId="28" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="45" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="44" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="43" operator="equal">
       <formula>"Low"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="44" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="45" operator="equal">
-      <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E32">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="26" operator="equal">
       <formula>"Low"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
-      <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="119">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="119">
       <formula>LEN(TRIM(E34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E35">
-    <cfRule type="cellIs" dxfId="21" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="116" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="117" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="118" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37:E38">
-    <cfRule type="cellIs" dxfId="18" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="90" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="89" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="90" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="91" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="82">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="82">
       <formula>LEN(TRIM(E40))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40:E41">
-    <cfRule type="cellIs" dxfId="14" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="79" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="80" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="81" operator="equal">
       <formula>"High"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
-      <formula>"Groupe UI"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"Groupe UI"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
-      <formula>"Groupe UI"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
-      <formula>"Terminé(e)"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
-      <formula>"En cours"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
-      <formula>"À faire"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"Abandonné"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
-      <formula>"À tester"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"High"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Groupe UI"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
<- STRUCTURE BACK END ->
</commit_message>
<xml_diff>
--- a/ShopConnect_Echeancier.xlsx
+++ b/ShopConnect_Echeancier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ShopConnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D64EAA-6289-4160-A944-0BCF72082E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626DBF0E-F83B-48BE-B1B8-76D00EDE83E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
   <si>
     <t>Tâches</t>
   </si>
@@ -296,10 +296,10 @@
     <t>Préparation finale et ajustements avant la présentation</t>
   </si>
   <si>
-    <t>En attente de Validation de la part du professeur</t>
-  </si>
-  <si>
     <t>Création des services pour les utilisateurs, produits, et boutiques</t>
+  </si>
+  <si>
+    <t>En attente de Retour de Mr Martel</t>
   </si>
 </sst>
 </file>
@@ -4091,8 +4091,8 @@
   <dimension ref="B1:I47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -4287,7 +4287,7 @@
         <v>45566</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4334,7 +4334,7 @@
         <v>45</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>9</v>
@@ -4345,10 +4345,10 @@
       <c r="G13" s="13">
         <v>45564</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="H13" s="13">
+        <v>45569</v>
+      </c>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="2:9" s="2" customFormat="1" ht="27.6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
@@ -4373,7 +4373,7 @@
         <v>45566</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4448,7 +4448,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>9</v>
@@ -4459,7 +4459,9 @@
       <c r="G18" s="13">
         <v>45571</v>
       </c>
-      <c r="H18" s="19"/>
+      <c r="H18" s="19">
+        <v>45570</v>
+      </c>
       <c r="I18" s="20" t="s">
         <v>51</v>
       </c>
@@ -4481,10 +4483,10 @@
         <v>52</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>9</v>
@@ -4508,7 +4510,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E21" s="40" t="s">
         <v>9</v>
@@ -4544,7 +4546,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E23" s="28" t="s">
         <v>9</v>
@@ -4570,7 +4572,7 @@
       <c r="H24" s="19"/>
       <c r="I24" s="42"/>
     </row>
-    <row r="25" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>30</v>
       </c>
@@ -4582,7 +4584,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="2:9" s="2" customFormat="1" ht="28.2" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" s="2" customFormat="1" ht="28.2" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="43" t="s">
         <v>57</v>
       </c>
@@ -4590,7 +4592,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>9</v>
@@ -4601,12 +4603,14 @@
       <c r="G26" s="13">
         <v>45592</v>
       </c>
-      <c r="H26" s="13"/>
+      <c r="H26" s="13">
+        <v>45570</v>
+      </c>
       <c r="I26" s="36" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B27" s="30" t="s">
         <v>31</v>
       </c>
@@ -4618,7 +4622,7 @@
       <c r="H27" s="32"/>
       <c r="I27" s="33"/>
     </row>
-    <row r="28" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B28" s="35" t="s">
         <v>60</v>
       </c>
@@ -4626,7 +4630,7 @@
         <v>61</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>9</v>
@@ -4642,7 +4646,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="2:9" s="2" customFormat="1" ht="42" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" s="2" customFormat="1" ht="42" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="37" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Mise à jour complète du code dans la branche back_up
</commit_message>
<xml_diff>
--- a/ShopConnect_Echeancier.xlsx
+++ b/ShopConnect_Echeancier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ShopConnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626DBF0E-F83B-48BE-B1B8-76D00EDE83E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0734C66B-54CB-4D23-A0EA-8B6D4E6129ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
   <si>
     <t>Tâches</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>En attente de Retour de Mr Martel</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -365,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,8 +401,40 @@
         </stop>
       </gradientFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <gradientFill degree="180">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFFC000"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <gradientFill degree="180">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFF0000"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -556,15 +591,6 @@
       <bottom style="hair">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="mediumDashDot">
-        <color rgb="FF92D050"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -764,19 +790,13 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,7 +811,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -800,40 +820,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -847,6 +861,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,7 +952,25 @@
     <dxf>
       <font>
         <b/>
+        <color rgb="FFFF9900"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -944,6 +988,23 @@
     <dxf>
       <font>
         <b/>
+        <color rgb="FF34A853"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FFFF0000"/>
       </font>
       <fill>
@@ -970,7 +1031,17 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF00FFFF"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF9900"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -987,6 +1058,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF00FFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <color rgb="FFFF9900"/>
       </font>
@@ -997,15 +1093,6 @@
     <dxf>
       <font>
         <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <color rgb="FF34A853"/>
       </font>
       <fill>
@@ -1014,8 +1101,17 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color rgb="FFFF9900"/>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -1032,33 +1128,33 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF00FFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF34A853"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF9900"/>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FF000000"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -1075,6 +1171,22 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <u/>
         <color rgb="FF1155CC"/>
       </font>
@@ -1118,6 +1230,15 @@
     </dxf>
     <dxf>
       <font>
+        <u/>
+        <color rgb="FF1155CC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike/>
         <color rgb="FF000000"/>
       </font>
@@ -1136,6 +1257,14 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF00FF00"/>
       </font>
       <fill>
@@ -1153,7 +1282,33 @@
     </dxf>
     <dxf>
       <font>
+        <strike/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00FF00"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -1188,6 +1343,14 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFF1C232"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF00FF00"/>
       </font>
       <fill>
@@ -1196,7 +1359,8 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFF1C232"/>
+        <u/>
+        <color rgb="FF1155CC"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -1206,22 +1370,6 @@
       <font>
         <strike/>
         <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -1231,128 +1379,6 @@
       <font>
         <b/>
         <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00FF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF1C232"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u/>
-        <color rgb="FF1155CC"/>
       </font>
       <fill>
         <patternFill patternType="none"/>
@@ -4090,9 +4116,8 @@
   </sheetPr>
   <dimension ref="B1:I47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -4108,45 +4133,45 @@
     <col min="9" max="9" width="44.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="51" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="52" t="s">
+    <row r="1" spans="2:9" s="47" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
     </row>
     <row r="2" spans="2:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="I2" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" collapsed="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>39</v>
       </c>
@@ -4158,7 +4183,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="2:9" s="2" customFormat="1" ht="13.8" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" s="2" customFormat="1" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
@@ -4174,7 +4199,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>24</v>
       </c>
@@ -4186,7 +4211,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:9" s="2" customFormat="1" ht="14.4" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" s="2" customFormat="1" ht="14.4" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
@@ -4202,19 +4227,19 @@
       <c r="H6" s="6"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B7" s="30" t="s">
+    <row r="7" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
     </row>
-    <row r="8" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
@@ -4238,7 +4263,7 @@
       </c>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="2:9" s="2" customFormat="1" ht="27.6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" s="2" customFormat="1" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>44</v>
       </c>
@@ -4264,7 +4289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:9" s="2" customFormat="1" ht="27.6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" s="2" customFormat="1" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>15</v>
       </c>
@@ -4290,7 +4315,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" collapsed="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>26</v>
       </c>
@@ -4302,7 +4327,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>41</v>
       </c>
@@ -4326,7 +4351,7 @@
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="2:9" s="2" customFormat="1" ht="27.6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" s="2" customFormat="1" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>44</v>
       </c>
@@ -4350,7 +4375,7 @@
       </c>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="2:9" s="2" customFormat="1" ht="27.6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" s="2" customFormat="1" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>15</v>
       </c>
@@ -4376,7 +4401,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" collapsed="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>27</v>
       </c>
@@ -4388,7 +4413,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="2:9" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" s="2" customFormat="1" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>44</v>
       </c>
@@ -4410,11 +4435,9 @@
       <c r="H16" s="13">
         <v>45568</v>
       </c>
-      <c r="I16" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="2:9" s="2" customFormat="1" ht="27.6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" s="2" customFormat="1" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>46</v>
       </c>
@@ -4440,7 +4463,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
         <v>49</v>
       </c>
@@ -4467,7 +4490,7 @@
       </c>
     </row>
     <row r="19" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="8"/>
@@ -4476,17 +4499,17 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="47"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="33" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>9</v>
@@ -4497,40 +4520,44 @@
       <c r="G20" s="13">
         <v>45571</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="36" t="s">
+      <c r="H20" s="13">
+        <v>45580</v>
+      </c>
+      <c r="I20" s="34" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:9" s="2" customFormat="1" ht="42" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="41">
+      <c r="D21" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="39">
         <v>45565</v>
       </c>
-      <c r="G21" s="41">
-        <v>45571</v>
-      </c>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42" t="s">
+      <c r="G21" s="39">
+        <v>45587</v>
+      </c>
+      <c r="H21" s="39">
+        <v>45587</v>
+      </c>
+      <c r="I21" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -4538,45 +4565,45 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" s="2" customFormat="1" ht="42" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="29">
+      <c r="D23" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="27">
         <v>45579</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="27">
         <v>45592</v>
       </c>
-      <c r="H23" s="29"/>
-      <c r="I23" s="36" t="s">
+      <c r="H23" s="27"/>
+      <c r="I23" s="34" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:9" s="2" customFormat="1" ht="14.4" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="48"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="16"/>
       <c r="D24" s="17"/>
       <c r="E24" s="18"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
-      <c r="I24" s="42"/>
+      <c r="I24" s="40"/>
     </row>
     <row r="25" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -4584,15 +4611,15 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="2:9" s="2" customFormat="1" ht="28.2" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="43" t="s">
+    <row r="26" spans="2:9" s="2" customFormat="1" ht="27.6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="41" t="s">
         <v>57</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>9</v>
@@ -4606,31 +4633,31 @@
       <c r="H26" s="13">
         <v>45570</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="33"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="33" t="s">
         <v>60</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>61</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>9</v>
@@ -4642,48 +4669,48 @@
         <v>45599</v>
       </c>
       <c r="H28" s="13"/>
-      <c r="I28" s="36" t="s">
+      <c r="I28" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="2:9" s="2" customFormat="1" ht="42" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D29" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="41">
+      <c r="F29" s="39">
         <v>45593</v>
       </c>
-      <c r="G29" s="41">
+      <c r="G29" s="39">
         <v>45599</v>
       </c>
-      <c r="H29" s="41"/>
-      <c r="I29" s="42" t="s">
+      <c r="H29" s="39"/>
+      <c r="I29" s="40" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="30" t="s">
+    <row r="30" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B30" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="33"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="31"/>
     </row>
-    <row r="31" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="44" t="s">
+    <row r="31" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="42" t="s">
         <v>66</v>
       </c>
       <c r="C31" s="21" t="s">
@@ -4702,48 +4729,48 @@
         <v>45606</v>
       </c>
       <c r="H31" s="24"/>
-      <c r="I31" s="45" t="s">
+      <c r="I31" s="43" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:9" s="2" customFormat="1" ht="28.2" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="37" t="s">
+    <row r="32" spans="2:9" s="2" customFormat="1" ht="28.2" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="41">
+      <c r="F32" s="39">
         <v>45600</v>
       </c>
-      <c r="G32" s="41">
+      <c r="G32" s="39">
         <v>45606</v>
       </c>
-      <c r="H32" s="41"/>
-      <c r="I32" s="42" t="s">
+      <c r="H32" s="39"/>
+      <c r="I32" s="40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="30" t="s">
+    <row r="33" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B33" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="33"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="31"/>
     </row>
-    <row r="34" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="44" t="s">
+    <row r="34" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="42" t="s">
         <v>72</v>
       </c>
       <c r="C34" s="9" t="s">
@@ -4762,51 +4789,51 @@
         <v>45648</v>
       </c>
       <c r="H34" s="13"/>
-      <c r="I34" s="36" t="s">
+      <c r="I34" s="34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="2:9" s="2" customFormat="1" ht="14.4" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="37" t="s">
+    <row r="35" spans="2:9" s="2" customFormat="1" ht="14.4" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="38"/>
-      <c r="D35" s="39" t="s">
+      <c r="C35" s="36"/>
+      <c r="D35" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="34">
+      <c r="F35" s="32">
         <v>45607</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="32">
         <v>45613</v>
       </c>
-      <c r="H35" s="41"/>
-      <c r="I35" s="42"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="40"/>
     </row>
-    <row r="36" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="30" t="s">
+    <row r="36" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B36" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="33"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="31"/>
     </row>
-    <row r="37" spans="2:9" s="2" customFormat="1" ht="41.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="35" t="s">
+    <row r="37" spans="2:9" s="2" customFormat="1" ht="41.4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="33" t="s">
         <v>75</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>76</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>9</v>
@@ -4818,44 +4845,44 @@
         <v>45620</v>
       </c>
       <c r="H37" s="13"/>
-      <c r="I37" s="36" t="s">
+      <c r="I37" s="34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="2:9" s="2" customFormat="1" ht="28.2" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="37" t="s">
+    <row r="38" spans="2:9" s="2" customFormat="1" ht="28.2" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="39" t="s">
+      <c r="C38" s="36"/>
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F38" s="39">
         <v>45614</v>
       </c>
-      <c r="G38" s="41">
+      <c r="G38" s="39">
         <v>45648</v>
       </c>
-      <c r="H38" s="41"/>
-      <c r="I38" s="42"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="40"/>
     </row>
     <row r="39" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="33"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="31"/>
     </row>
     <row r="40" spans="2:9" s="2" customFormat="1" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -4874,129 +4901,129 @@
         <v>45634</v>
       </c>
       <c r="H40" s="13"/>
-      <c r="I40" s="36" t="s">
+      <c r="I40" s="34" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" spans="2:9" s="2" customFormat="1" ht="14.4" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="37"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="39" t="s">
+      <c r="B41" s="35"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="42"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="40"/>
     </row>
     <row r="42" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="33"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="31"/>
     </row>
     <row r="43" spans="2:9" s="2" customFormat="1" ht="28.2" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="40" t="s">
+      <c r="E43" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="41">
+      <c r="F43" s="39">
         <v>45621</v>
       </c>
-      <c r="G43" s="41">
+      <c r="G43" s="39">
         <v>45634</v>
       </c>
-      <c r="H43" s="41"/>
-      <c r="I43" s="42" t="s">
+      <c r="H43" s="39"/>
+      <c r="I43" s="40" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="44" spans="2:9" s="2" customFormat="1" ht="18" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="33"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="31"/>
     </row>
     <row r="45" spans="2:9" s="2" customFormat="1" ht="42" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="38" t="s">
+      <c r="C45" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="39" t="s">
+      <c r="D45" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="40" t="s">
+      <c r="E45" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F45" s="41">
+      <c r="F45" s="39">
         <v>37599</v>
       </c>
-      <c r="G45" s="41">
+      <c r="G45" s="39">
         <v>45648</v>
       </c>
-      <c r="H45" s="41"/>
-      <c r="I45" s="42" t="s">
+      <c r="H45" s="39"/>
+      <c r="I45" s="40" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="46" spans="2:9" s="2" customFormat="1" ht="17.399999999999999" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="33"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="31"/>
     </row>
     <row r="47" spans="2:9" s="2" customFormat="1" ht="42" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="39" t="s">
+      <c r="D47" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E47" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="41">
+      <c r="F47" s="39">
         <v>45642</v>
       </c>
-      <c r="G47" s="41">
+      <c r="G47" s="39">
         <v>45648</v>
       </c>
-      <c r="H47" s="41"/>
-      <c r="I47" s="42" t="s">
+      <c r="H47" s="39"/>
+      <c r="I47" s="40" t="s">
         <v>86</v>
       </c>
     </row>
@@ -5044,7 +5071,7 @@
       <formula>"Groupe UI"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2 D4 D6 D8:D10 D12:D14 D16:D18 D20:D21 D23:D24 D26">
+  <conditionalFormatting sqref="D2 D4 D6 D8:D10 D26 D23:D24 D12:D21">
     <cfRule type="cellIs" dxfId="59" priority="143" operator="equal">
       <formula>"Terminé(e)"</formula>
     </cfRule>
@@ -5052,43 +5079,43 @@
       <formula>"En cours"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 D6 D8:D10 D12:D14 D16:D18 D20:D21 D23:D24 D26">
-    <cfRule type="cellIs" dxfId="57" priority="147" operator="equal">
-      <formula>"À tester"</formula>
+  <conditionalFormatting sqref="D4 D6 D8:D10 D26 D23:D24 D12:D21">
+    <cfRule type="cellIs" dxfId="57" priority="145" operator="equal">
+      <formula>"À faire"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="56" priority="146" operator="equal">
       <formula>"Abandonné"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="145" operator="equal">
-      <formula>"À faire"</formula>
+    <cfRule type="cellIs" dxfId="55" priority="147" operator="equal">
+      <formula>"À tester"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D29 D45 D47">
-    <cfRule type="cellIs" dxfId="54" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="38" operator="equal">
+      <formula>"Terminé(e)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="39" operator="equal">
       <formula>"En cours"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="40" operator="equal">
       <formula>"À faire"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
       <formula>"Abandonné"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="42" operator="equal">
       <formula>"À tester"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="38" operator="equal">
-      <formula>"Terminé(e)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D32">
-    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="21" operator="equal">
+      <formula>"Terminé(e)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="22" operator="equal">
+      <formula>"En cours"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
       <formula>"À faire"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="21" operator="equal">
-      <formula>"Terminé(e)"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="22" operator="equal">
-      <formula>"En cours"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
       <formula>"Abandonné"</formula>
@@ -5098,28 +5125,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:D35">
-    <cfRule type="cellIs" dxfId="44" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="111" operator="equal">
+      <formula>"Terminé(e)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="112" operator="equal">
+      <formula>"En cours"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="113" operator="equal">
+      <formula>"À faire"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="114" operator="equal">
+      <formula>"Abandonné"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="115" operator="equal">
       <formula>"À tester"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="113" operator="equal">
-      <formula>"À faire"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="111" operator="equal">
-      <formula>"Terminé(e)"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="112" operator="equal">
-      <formula>"En cours"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="114" operator="equal">
-      <formula>"Abandonné"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D38">
-    <cfRule type="cellIs" dxfId="39" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="84" operator="equal">
+      <formula>"Terminé(e)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="85" operator="equal">
       <formula>"En cours"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="84" operator="equal">
-      <formula>"Terminé(e)"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="37" priority="86" operator="equal">
       <formula>"À faire"</formula>
@@ -5132,20 +5159,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:D41">
-    <cfRule type="cellIs" dxfId="34" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="74" operator="equal">
+      <formula>"Terminé(e)"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="75" operator="equal">
       <formula>"En cours"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="76" operator="equal">
+      <formula>"À faire"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="77" operator="equal">
+      <formula>"Abandonné"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="78" operator="equal">
       <formula>"À tester"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="74" operator="equal">
-      <formula>"Terminé(e)"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="76" operator="equal">
-      <formula>"À faire"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="77" operator="equal">
-      <formula>"Abandonné"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
@@ -5165,15 +5192,15 @@
       <formula>"À tester"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 E6 E8:E10 E12:E14 E16:E18 E20:E21 E23:E24 E26 E45 E47">
-    <cfRule type="cellIs" dxfId="24" priority="150" operator="equal">
-      <formula>"High"</formula>
+  <conditionalFormatting sqref="E4 E6 E8:E10 E26 E45 E47 E23:E24 E12:E21">
+    <cfRule type="cellIs" dxfId="24" priority="148" operator="equal">
+      <formula>"Low"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="23" priority="149" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="148" operator="equal">
-      <formula>"Low"</formula>
+    <cfRule type="cellIs" dxfId="22" priority="150" operator="equal">
+      <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10 E14">
@@ -5187,25 +5214,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E29">
-    <cfRule type="cellIs" dxfId="19" priority="45" operator="equal">
-      <formula>"High"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="43" operator="equal">
+      <formula>"Low"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="18" priority="44" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="43" operator="equal">
-      <formula>"Low"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="45" operator="equal">
+      <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E32">
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
-      <formula>"High"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
+      <formula>"Low"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="26" operator="equal">
-      <formula>"Low"</formula>
+    <cfRule type="cellIs" dxfId="14" priority="28" operator="equal">
+      <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
@@ -5225,11 +5252,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37:E38">
-    <cfRule type="cellIs" dxfId="9" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="89" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="90" operator="equal">
       <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="89" operator="equal">
-      <formula>"Low"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="7" priority="91" operator="equal">
       <formula>"High"</formula>
@@ -5263,18 +5290,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4 D16:D18 D8:D10 D45 D23:D24 D26 D34:D35 D28:D29 D40:D41 D37:D38 D43 D31:D32 D6 D20:D21 D47 D12:D14" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4 D12:D14 D8:D10 D45 D16:D18 D26 D34:D35 D28:D29 D40:D41 D37:D38 D43 D31:D32 D6 D20:D21 D47 D23:D24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"En cours,Terminé(e),À faire,À tester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4 E16:E18 E8:E10 E45 E23:E24 E26 E34:E35 E28:E29 E40:E41 E37:E38 E43 E31:E32 E6 E20:E21 E47 E12:E14" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4 E12:E14 E8:E10 E45 E16:E18 E26 E34:E35 E28:E29 E40:E41 E37:E38 E43 E31:E32 E6 E20:E21 E47 E23:E24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Low,High,Medium"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup paperSize="8" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <pageSetup paperSize="8" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
   <tableParts count="10">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -5284,6 +5310,7 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>